<commit_message>
workbook data parsing; new modular file structure
repo originally had everything in one massive file. I moved out as many
psuedoclassical structures and functions as possible into separate
require('') files. this makes for a much saner dev environment.

tests not passing, but they simply haven't been updated yet.
microsoft color numbers need to be converted to hex or rgb, otherwise
whole workbook is being correctly parsed for usable data.
</commit_message>
<xml_diff>
--- a/test/spreadsheets/excel_mac_2011-formatting.xlsx
+++ b/test/spreadsheets/excel_mac_2011-formatting.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-1520" windowWidth="25600" windowHeight="20720" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="19240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="first sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="first sheet" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Hey</t>
   </si>
@@ -39,6 +40,10 @@
   </si>
   <si>
     <t>second sheet</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>bob</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -493,40 +498,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27" ht="36">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -558,4 +548,45 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:27" ht="36">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>